<commit_message>
Bug fixes in bird_extended & early implementation of machine_code
</commit_message>
<xml_diff>
--- a/Logisim_Evolutionary_Sequence_of_CPUs/5.1-Bird_Extended/bird_extension_changes.xlsx
+++ b/Logisim_Evolutionary_Sequence_of_CPUs/5.1-Bird_Extended/bird_extension_changes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rsan\projects\school\CSE4117-Microprocessors\Project_2\Logisim\Bird_extended\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA2C4D21-D2C5-4DA1-9A9F-0820973F1066}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAC6B5BD-F307-47D8-A775-AEF21CE1252B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{DE8CB966-0C5E-436C-AC6F-D64CE43CCC0D}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="89">
   <si>
     <t>Address</t>
   </si>
@@ -294,6 +294,15 @@
   </si>
   <si>
     <t>0x9440</t>
+  </si>
+  <si>
+    <t>0x100E</t>
+  </si>
+  <si>
+    <t>0x1542F</t>
+  </si>
+  <si>
+    <t>0x800</t>
   </si>
 </sst>
 </file>
@@ -912,10 +921,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B17C1B6C-1DD3-447E-A634-9FBDC6E555DB}">
-  <dimension ref="C1:AN26"/>
+  <dimension ref="C1:AP26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="X28" sqref="X28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -928,7 +937,7 @@
     <col min="40" max="40" width="7.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="3:40" x14ac:dyDescent="0.25">
+    <row r="1" spans="3:42" x14ac:dyDescent="0.25">
       <c r="D1" s="19" t="s">
         <v>56</v>
       </c>
@@ -948,7 +957,7 @@
       <c r="R1" s="20"/>
       <c r="S1" s="20"/>
     </row>
-    <row r="2" spans="3:40" x14ac:dyDescent="0.25">
+    <row r="2" spans="3:42" x14ac:dyDescent="0.25">
       <c r="D2" s="20"/>
       <c r="E2" s="20"/>
       <c r="F2" s="20"/>
@@ -966,7 +975,7 @@
       <c r="R2" s="20"/>
       <c r="S2" s="20"/>
     </row>
-    <row r="3" spans="3:40" x14ac:dyDescent="0.25">
+    <row r="3" spans="3:42" x14ac:dyDescent="0.25">
       <c r="D3" s="20"/>
       <c r="E3" s="20"/>
       <c r="F3" s="20"/>
@@ -984,7 +993,7 @@
       <c r="R3" s="20"/>
       <c r="S3" s="20"/>
     </row>
-    <row r="8" spans="3:40" x14ac:dyDescent="0.25">
+    <row r="8" spans="3:42" x14ac:dyDescent="0.25">
       <c r="D8" s="18" t="s">
         <v>40</v>
       </c>
@@ -1012,7 +1021,7 @@
       <c r="AH8" s="18"/>
       <c r="AI8" s="18"/>
     </row>
-    <row r="9" spans="3:40" x14ac:dyDescent="0.25">
+    <row r="9" spans="3:42" x14ac:dyDescent="0.25">
       <c r="D9" s="5" t="s">
         <v>0</v>
       </c>
@@ -1113,7 +1122,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="10" spans="3:40" ht="63" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="3:42" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D10" s="5"/>
       <c r="E10" s="16" t="s">
         <v>20</v>
@@ -1207,7 +1216,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="11" spans="3:40" x14ac:dyDescent="0.25">
+    <row r="11" spans="3:42" x14ac:dyDescent="0.25">
       <c r="C11" s="13" t="s">
         <v>20</v>
       </c>
@@ -1268,8 +1277,11 @@
       <c r="AN11" s="7" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="12" spans="3:40" x14ac:dyDescent="0.25">
+      <c r="AP11" s="10" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="12" spans="3:42" x14ac:dyDescent="0.25">
       <c r="C12" s="13" t="s">
         <v>57</v>
       </c>
@@ -1334,8 +1346,11 @@
       <c r="AN12" s="9" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="13" spans="3:40" x14ac:dyDescent="0.25">
+      <c r="AP12" s="10" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="13" spans="3:42" x14ac:dyDescent="0.25">
       <c r="C13" s="13" t="s">
         <v>58</v>
       </c>
@@ -1400,8 +1415,11 @@
       <c r="AN13" s="7" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="14" spans="3:40" x14ac:dyDescent="0.25">
+      <c r="AP13" s="10" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="14" spans="3:42" x14ac:dyDescent="0.25">
       <c r="C14" s="13" t="s">
         <v>59</v>
       </c>
@@ -1462,8 +1480,11 @@
       <c r="AN14" s="9" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="15" spans="3:40" x14ac:dyDescent="0.25">
+      <c r="AP14" s="10" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="15" spans="3:42" x14ac:dyDescent="0.25">
       <c r="C15" s="13" t="s">
         <v>60</v>
       </c>
@@ -1516,8 +1537,11 @@
       <c r="AN15" s="7" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="16" spans="3:40" x14ac:dyDescent="0.25">
+      <c r="AP15" s="10" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="16" spans="3:42" x14ac:dyDescent="0.25">
       <c r="C16" s="13" t="s">
         <v>61</v>
       </c>
@@ -1574,8 +1598,11 @@
       <c r="AN16" s="9" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="17" spans="3:40" x14ac:dyDescent="0.25">
+      <c r="AP16" s="10" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="17" spans="3:42" x14ac:dyDescent="0.25">
       <c r="C17" s="13"/>
       <c r="D17" s="4">
         <v>6</v>
@@ -1624,8 +1651,11 @@
       <c r="AN17" s="7" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="18" spans="3:40" x14ac:dyDescent="0.25">
+      <c r="AP17" s="10" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="18" spans="3:42" x14ac:dyDescent="0.25">
       <c r="C18" s="13" t="s">
         <v>66</v>
       </c>
@@ -1686,8 +1716,11 @@
       <c r="AN18" s="9" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="19" spans="3:40" x14ac:dyDescent="0.25">
+      <c r="AP18" s="10" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="19" spans="3:42" x14ac:dyDescent="0.25">
       <c r="C19" s="13" t="s">
         <v>65</v>
       </c>
@@ -1752,8 +1785,11 @@
       <c r="AN19" s="7" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="20" spans="3:40" x14ac:dyDescent="0.25">
+      <c r="AP19" s="10" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="20" spans="3:42" x14ac:dyDescent="0.25">
       <c r="C20" s="13" t="s">
         <v>64</v>
       </c>
@@ -1807,8 +1843,11 @@
       <c r="AN20" s="9" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="21" spans="3:40" x14ac:dyDescent="0.25">
+      <c r="AP20" s="10" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="21" spans="3:42" x14ac:dyDescent="0.25">
       <c r="C21" s="13" t="s">
         <v>63</v>
       </c>
@@ -1878,8 +1917,11 @@
       <c r="AN21" s="7" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="22" spans="3:40" x14ac:dyDescent="0.25">
+      <c r="AP21" s="10" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="22" spans="3:42" x14ac:dyDescent="0.25">
       <c r="C22" s="13" t="s">
         <v>62</v>
       </c>
@@ -1933,8 +1975,11 @@
       <c r="AN22" s="9" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="23" spans="3:40" x14ac:dyDescent="0.25">
+      <c r="AP22" s="10" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="23" spans="3:42" x14ac:dyDescent="0.25">
       <c r="C23" s="13" t="s">
         <v>68</v>
       </c>
@@ -1996,8 +2041,11 @@
       <c r="AN23" s="7" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="24" spans="3:40" x14ac:dyDescent="0.25">
+      <c r="AP23" s="10" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="24" spans="3:42" x14ac:dyDescent="0.25">
       <c r="C24" s="13" t="s">
         <v>67</v>
       </c>
@@ -2063,8 +2111,11 @@
       <c r="AN24" s="9" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="25" spans="3:40" x14ac:dyDescent="0.25">
+      <c r="AP24" s="10" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="25" spans="3:42" x14ac:dyDescent="0.25">
       <c r="D25" s="1"/>
       <c r="X25" s="13" t="s">
         <v>70</v>
@@ -2091,8 +2142,11 @@
       <c r="AN25" s="7" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="26" spans="3:40" x14ac:dyDescent="0.25">
+      <c r="AP25" s="10" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="26" spans="3:42" x14ac:dyDescent="0.25">
       <c r="X26" s="13" t="s">
         <v>72</v>
       </c>
@@ -2117,6 +2171,9 @@
       <c r="AM26" s="14"/>
       <c r="AN26" s="13" t="s">
         <v>39</v>
+      </c>
+      <c r="AP26" s="10" t="s">
+        <v>88</v>
       </c>
     </row>
   </sheetData>
@@ -2737,6 +2794,13 @@
     </row>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="C6:I6"/>
+    <mergeCell ref="W6:AC6"/>
+    <mergeCell ref="C13:I13"/>
+    <mergeCell ref="W13:AC13"/>
+    <mergeCell ref="C8:F8"/>
+    <mergeCell ref="G8:R8"/>
+    <mergeCell ref="W8:Z8"/>
     <mergeCell ref="AA22:AL22"/>
     <mergeCell ref="W23:AL23"/>
     <mergeCell ref="C3:R3"/>
@@ -2753,13 +2817,6 @@
     <mergeCell ref="W16:AL16"/>
     <mergeCell ref="AA8:AL8"/>
     <mergeCell ref="W9:AL9"/>
-    <mergeCell ref="C6:I6"/>
-    <mergeCell ref="W6:AC6"/>
-    <mergeCell ref="C13:I13"/>
-    <mergeCell ref="W13:AC13"/>
-    <mergeCell ref="C8:F8"/>
-    <mergeCell ref="G8:R8"/>
-    <mergeCell ref="W8:Z8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>